<commit_message>
Tested different ks for PCA and FLD reduced
Tested k from 5 to 250, increments of 5
</commit_message>
<xml_diff>
--- a/accuracies.xlsx
+++ b/accuracies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alec\Documents\Git\utk\ece471\fashion-mnist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F744F9C6-E03A-4A45-83B0-D44F1E7E3A52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA538183-45E4-4DC2-9D78-C2E86D665C0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{E38AB83A-E29C-4C62-844C-6AADFEF943B5}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
   <si>
     <t>FLD</t>
   </si>
@@ -57,6 +57,21 @@
   </si>
   <si>
     <t>10-fold CV</t>
+  </si>
+  <si>
+    <t>[0.8203 0.8263 0.8273 0.8291 0.8293 0.8295 0.8291 0.8292 0.8288 0.8288</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.8281 0.8278 0.8281 0.8284 0.8287 0.8281 0.8273 0.8265 0.8271 0.8263</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.8261 0.8253 0.8254 0.8256 0.8252 0.8256 0.8257 0.826  0.8254 0.825</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.8249 0.825  0.8246 0.8245 0.8239 0.8232 0.8235 0.8237 0.8236 0.8237</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.8234 0.8233 0.8235 0.8228 0.8231 0.8233 0.8227 0.8228 0.8227 0.8221]</t>
   </si>
 </sst>
 </file>
@@ -408,9 +423,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D19BCC-073D-453D-A3D7-EF352F1A7484}">
-  <dimension ref="B1:E15"/>
+  <dimension ref="B1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -554,6 +571,126 @@
         <v>0.81699999999999995</v>
       </c>
     </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>15</v>
+      </c>
+      <c r="G19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0.85540000000000005</v>
+      </c>
+      <c r="E20">
+        <v>0.85150000000000003</v>
+      </c>
+      <c r="F20">
+        <v>0.84619999999999995</v>
+      </c>
+      <c r="G20">
+        <v>0.84150000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0.86029999999999995</v>
+      </c>
+      <c r="E21">
+        <v>0.8619</v>
+      </c>
+      <c r="F21">
+        <v>0.85650000000000004</v>
+      </c>
+      <c r="G21">
+        <v>0.85409999999999997</v>
+      </c>
+      <c r="I21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0.82030000000000003</v>
+      </c>
+      <c r="E29">
+        <v>0.82630000000000003</v>
+      </c>
+      <c r="F29">
+        <v>0.82730000000000004</v>
+      </c>
+      <c r="G29">
+        <v>0.82909999999999995</v>
+      </c>
+      <c r="I29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tested a basic CNN with testing and decision trees with m-fold and the test set. Used division by 255 for normalizing
</commit_message>
<xml_diff>
--- a/accuracies.xlsx
+++ b/accuracies.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alec\Documents\Git\utk\ece471\fashion-mnist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carl\Desktop\College\ECE471\final_project\Repo\fashion-mnist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA538183-45E4-4DC2-9D78-C2E86D665C0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936CB23C-9EFF-45FB-AF1D-45F2847AA80F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{E38AB83A-E29C-4C62-844C-6AADFEF943B5}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
   <si>
     <t>FLD</t>
   </si>
@@ -72,6 +72,33 @@
   </si>
   <si>
     <t xml:space="preserve"> 0.8234 0.8233 0.8235 0.8228 0.8231 0.8233 0.8227 0.8228 0.8227 0.8221]</t>
+  </si>
+  <si>
+    <t>Carl</t>
+  </si>
+  <si>
+    <t>Normalized</t>
+  </si>
+  <si>
+    <t>(Divide by 255)</t>
+  </si>
+  <si>
+    <t>Basic CNN</t>
+  </si>
+  <si>
+    <t>Acc</t>
+  </si>
+  <si>
+    <t>Loss</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>M-fold (training data only)</t>
+  </si>
+  <si>
+    <t>92.48 with a random seed</t>
   </si>
 </sst>
 </file>
@@ -423,23 +450,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D19BCC-073D-453D-A3D7-EF352F1A7484}">
-  <dimension ref="B1:I33"/>
+  <dimension ref="B1:V33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>7</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -450,7 +480,7 @@
         <v>0.85150000000000003</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>4</v>
       </c>
@@ -461,7 +491,7 @@
         <v>0.68600000000000005</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -472,7 +502,7 @@
         <v>0.82420000000000004</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -483,7 +513,15 @@
         <v>0.72789999999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -493,8 +531,14 @@
       <c r="D7">
         <v>0.8619</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="T7" t="s">
+        <v>18</v>
+      </c>
+      <c r="V7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>4</v>
       </c>
@@ -504,8 +548,17 @@
       <c r="E8">
         <v>0.68500000000000005</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="R8" t="s">
+        <v>17</v>
+      </c>
+      <c r="T8">
+        <v>92.23</v>
+      </c>
+      <c r="V8">
+        <v>0.21990000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>5</v>
       </c>
@@ -515,8 +568,11 @@
       <c r="E9">
         <v>0.80300000000000005</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="T9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>6</v>
       </c>
@@ -527,7 +583,7 @@
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -538,7 +594,7 @@
         <v>0.82630000000000003</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>4</v>
       </c>
@@ -549,7 +605,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>5</v>
       </c>
@@ -560,7 +616,7 @@
         <v>0.83199999999999996</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>6</v>
       </c>
@@ -571,7 +627,7 @@
         <v>0.81699999999999995</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>5</v>
       </c>
@@ -585,7 +641,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -604,8 +660,17 @@
       <c r="G20">
         <v>0.84150000000000003</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="R20" t="s">
+        <v>20</v>
+      </c>
+      <c r="T20" t="s">
+        <v>7</v>
+      </c>
+      <c r="U20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -627,28 +692,34 @@
       <c r="I21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="T21">
+        <v>79.25</v>
+      </c>
+      <c r="U21">
+        <v>79.52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="I25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>0</v>
       </c>
@@ -671,17 +742,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="I30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="I31" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="I32" t="s">
         <v>12</v>
       </c>

</xml_diff>